<commit_message>
Report data & plot
</commit_message>
<xml_diff>
--- a/data/testdrivedata/driving_info_from_dashcam.xlsx
+++ b/data/testdrivedata/driving_info_from_dashcam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\폴더 모음\학업 &amp; 학교 (대학원)\수업\3학기\AE 6505\project\data\I85\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\폴더 모음\학업 &amp; 학교 (대학원)\수업\3학기\AE 6505\project\lane_project\data\testdrivedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC19F08-0831-4456-AAF3-29BE657D0548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9CF538-268C-4CCE-B281-4CC84D9187BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="phase 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="46">
   <si>
     <t>lane change time</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -177,6 +177,38 @@
   </si>
   <si>
     <t>end(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>estimation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overshoot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Undershoot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -505,32 +537,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D5:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>30</v>
       </c>
@@ -543,8 +577,11 @@
       <c r="G8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D9" s="1">
         <v>0.38946759259259256</v>
       </c>
@@ -555,7 +592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E10" s="1">
         <v>0.39054398148148151</v>
       </c>
@@ -566,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E11" s="1">
         <v>0.39082175925925927</v>
       </c>
@@ -574,44 +611,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E12" s="1">
         <v>0.39199074074074075</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E13" s="1">
         <v>0.39351851851851855</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E14" s="1">
         <v>0.39406249999999998</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E15" s="1">
         <v>0.39424768518518521</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E16" s="1">
         <v>0.39436342592592594</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.3">
@@ -621,6 +676,9 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E18" s="1">
@@ -629,6 +687,12 @@
       <c r="F18" t="s">
         <v>9</v>
       </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E19" s="1">
@@ -637,6 +701,12 @@
       <c r="F19" t="s">
         <v>8</v>
       </c>
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E20" s="1">
@@ -645,6 +715,12 @@
       <c r="F20" t="s">
         <v>9</v>
       </c>
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E21" s="1">
@@ -653,6 +729,9 @@
       <c r="F21" t="s">
         <v>12</v>
       </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E22" s="1">
@@ -661,6 +740,9 @@
       <c r="F22" t="s">
         <v>6</v>
       </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E23" s="1">
@@ -669,6 +751,9 @@
       <c r="F23" t="s">
         <v>8</v>
       </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E24" s="1">
@@ -677,6 +762,9 @@
       <c r="F24" t="s">
         <v>11</v>
       </c>
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E25" s="1">
@@ -685,6 +773,9 @@
       <c r="F25" t="s">
         <v>13</v>
       </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E26" s="1">
@@ -693,6 +784,12 @@
       <c r="F26" t="s">
         <v>14</v>
       </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.3">
@@ -702,6 +799,9 @@
       <c r="F27" t="s">
         <v>6</v>
       </c>
+      <c r="H27" t="s">
+        <v>39</v>
+      </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.3">
@@ -711,6 +811,9 @@
       <c r="F28" t="s">
         <v>8</v>
       </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.3">
@@ -720,6 +823,9 @@
       <c r="G29" t="s">
         <v>15</v>
       </c>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.3">
@@ -729,6 +835,9 @@
       <c r="G30" t="s">
         <v>16</v>
       </c>
+      <c r="H30" t="s">
+        <v>40</v>
+      </c>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.3">
@@ -738,6 +847,9 @@
       <c r="G31" t="s">
         <v>17</v>
       </c>
+      <c r="H31" t="s">
+        <v>39</v>
+      </c>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.3">
@@ -747,6 +859,12 @@
       <c r="F32" t="s">
         <v>12</v>
       </c>
+      <c r="H32" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" t="s">
+        <v>43</v>
+      </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.3">
@@ -756,6 +874,9 @@
       <c r="F33" t="s">
         <v>18</v>
       </c>
+      <c r="H33" t="s">
+        <v>39</v>
+      </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.3">
@@ -764,6 +885,9 @@
       </c>
       <c r="G34" t="s">
         <v>19</v>
+      </c>
+      <c r="H34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.3">
@@ -783,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB0BFC-3A86-4063-9E63-29DE36BF385A}">
-  <dimension ref="D6:G43"/>
+  <dimension ref="D6:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -797,12 +921,12 @@
     <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>30</v>
       </c>
@@ -816,7 +940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D8" s="1">
         <v>0.40570601851851856</v>
       </c>
@@ -827,127 +951,175 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E9" s="1">
         <v>0.40593750000000001</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E10" s="1">
         <v>0.40704861111111112</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E11" s="1">
         <v>0.40825231481481478</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E12" s="1">
         <v>0.40837962962962965</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E13" s="1">
         <v>0.40880787037037036</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E14" s="1">
         <v>0.40900462962962963</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E15" s="1">
         <v>0.40909722222222222</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E16" s="1">
         <v>0.40953703703703703</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E17" s="1">
         <v>0.41059027777777773</v>
       </c>
       <c r="F17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E18" s="1">
         <v>0.41142361111111114</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E19" s="1">
         <v>0.4114814814814815</v>
       </c>
       <c r="G19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E20" s="1">
         <v>0.41399305555555554</v>
       </c>
       <c r="G20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E21" s="1">
         <v>0.41403935185185187</v>
       </c>
       <c r="F21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E22" s="1">
         <v>0.4142824074074074</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E23" s="1">
         <v>0.41469907407407408</v>
       </c>
       <c r="F23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
       <c r="E24" s="1">
         <v>0.4148958333333333</v>
       </c>
@@ -955,7 +1127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>31</v>
       </c>
@@ -966,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D27" s="1">
         <v>0.40587962962962965</v>
       </c>
@@ -976,8 +1148,11 @@
       <c r="F27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D28" s="1">
         <v>0.40593750000000001</v>
       </c>
@@ -987,8 +1162,11 @@
       <c r="F28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D29" s="1">
         <v>0.40704861111111112</v>
       </c>
@@ -998,8 +1176,11 @@
       <c r="F29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D30" s="1">
         <v>0.40825231481481478</v>
       </c>
@@ -1009,8 +1190,11 @@
       <c r="F30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D31" s="1">
         <v>0.40837962962962965</v>
       </c>
@@ -1021,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D32" s="1">
         <v>0.40880787037037036</v>
       </c>
@@ -1031,8 +1215,11 @@
       <c r="F32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D33" s="1">
         <v>0.40900462962962963</v>
       </c>
@@ -1043,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D34" s="1">
         <v>0.40909722222222222</v>
       </c>
@@ -1054,7 +1241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D35" s="1">
         <v>0.40953703703703703</v>
       </c>
@@ -1065,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D36" s="1">
         <v>0.41059027777777773</v>
       </c>
@@ -1076,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D37" s="1">
         <v>0.41142361111111114</v>
       </c>
@@ -1087,7 +1274,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D38" s="1">
         <v>0.4114814814814815</v>
       </c>
@@ -1097,8 +1284,11 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D39" s="1">
         <v>0.41399305555555554</v>
       </c>
@@ -1109,7 +1299,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D40" s="1">
         <v>0.41403935185185187</v>
       </c>
@@ -1120,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D41" s="1">
         <v>0.4142824074074074</v>
       </c>
@@ -1131,7 +1321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D42" s="1">
         <v>0.41469907407407408</v>
       </c>
@@ -1142,7 +1332,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D43" s="1">
         <v>0.4148958333333333</v>
       </c>

</xml_diff>